<commit_message>
changes in the test steps
</commit_message>
<xml_diff>
--- a/DroneDeliverySystem_Test/DroneDeliverySystem_TestScenarios&TestCases_V1.xlsx
+++ b/DroneDeliverySystem_Test/DroneDeliverySystem_TestScenarios&TestCases_V1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahak\git\DroneDeliverySystem\DroneDeliverySystem_Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D809D20-536C-4BCD-B2EB-F48928359143}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81435AF-273C-4765-A148-3409EB6052CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" tabRatio="459" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" tabRatio="459" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestScenarios_FR" sheetId="6" r:id="rId1"/>
@@ -131,10 +131,6 @@
     <t>Validate that a processed list is generated that contains the orderId and dispatch time of the orders.</t>
   </si>
   <si>
-    <t xml:space="preserve">Validate that a schedule is generated in which the orders need to be delivered
-</t>
-  </si>
-  <si>
     <t>Validate that system is able to generate the NPS Score for the schedule created</t>
   </si>
   <si>
@@ -612,6 +608,10 @@
   </si>
   <si>
     <t xml:space="preserve">1) check that system generates the output file on diferrent Osperating System
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate that output file is generated containing the schedule in which the orders need to be delivered
 </t>
   </si>
 </sst>
@@ -1094,10 +1094,10 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1508,8 +1508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B768C5-55B0-4F80-B06C-2ACDAA19F2D0}">
   <dimension ref="B1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -1527,7 +1527,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" s="38"/>
     </row>
@@ -1536,7 +1536,7 @@
         <v>16</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" s="38"/>
     </row>
@@ -1545,7 +1545,7 @@
         <v>17</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" s="38"/>
     </row>
@@ -1587,7 +1587,7 @@
     </row>
     <row r="9" spans="2:6" ht="34" customHeight="1">
       <c r="B9" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>27</v>
@@ -1604,7 +1604,7 @@
     </row>
     <row r="10" spans="2:6" ht="34.5" customHeight="1">
       <c r="B10" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>28</v>
@@ -1619,10 +1619,10 @@
     </row>
     <row r="11" spans="2:6" ht="32" customHeight="1">
       <c r="B11" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>33</v>
@@ -1636,13 +1636,13 @@
     </row>
     <row r="12" spans="2:6" ht="33.5" customHeight="1">
       <c r="B12" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>35</v>
+        <v>178</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>25</v>
@@ -1653,26 +1653,26 @@
     </row>
     <row r="13" spans="2:6" ht="22.5" customHeight="1">
       <c r="B13" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>30</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="2:6" s="4" customFormat="1" ht="32" customHeight="1">
       <c r="B14" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>30</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>1</v>
@@ -1681,7 +1681,7 @@
     </row>
     <row r="15" spans="2:6" s="4" customFormat="1" ht="29" customHeight="1">
       <c r="B15" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>31</v>
@@ -1764,7 +1764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J345"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -2480,47 +2480,47 @@
       <c r="A1" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="42"/>
+      <c r="B1" s="41"/>
       <c r="C1" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="42"/>
+        <v>40</v>
+      </c>
+      <c r="D1" s="42"/>
+      <c r="E1" s="41"/>
       <c r="F1" s="40"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
       <c r="I1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="A2" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="41"/>
+      <c r="C2" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" s="41"/>
-      <c r="E2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="41"/>
       <c r="F2" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
       <c r="I2" s="32"/>
     </row>
     <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="42"/>
+      <c r="B3" s="41"/>
       <c r="C3" s="40"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="41"/>
       <c r="F3" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
       <c r="I3" s="33"/>
     </row>
     <row r="4" spans="1:10" ht="16" thickBot="1">
@@ -2554,22 +2554,22 @@
     </row>
     <row r="5" spans="1:10" ht="62">
       <c r="A5" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="C5" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="E5" s="18" t="s">
+      <c r="F5" s="18" t="s">
         <v>65</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>66</v>
       </c>
       <c r="G5" s="18"/>
       <c r="H5" s="26"/>
@@ -2577,22 +2577,22 @@
     </row>
     <row r="6" spans="1:10" ht="62">
       <c r="A6" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>68</v>
-      </c>
       <c r="E6" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" s="18" t="s">
         <v>70</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>71</v>
       </c>
       <c r="G6" s="28"/>
       <c r="H6" s="29"/>
@@ -2600,22 +2600,22 @@
     </row>
     <row r="7" spans="1:10" ht="62">
       <c r="A7" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D7" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="E7" s="18" t="s">
-        <v>75</v>
-      </c>
       <c r="F7" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G7" s="28"/>
       <c r="H7" s="29"/>
@@ -2647,47 +2647,47 @@
       <c r="A10" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="42"/>
+      <c r="B10" s="41"/>
       <c r="C10" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="41"/>
-      <c r="E10" s="42"/>
+        <v>41</v>
+      </c>
+      <c r="D10" s="42"/>
+      <c r="E10" s="41"/>
       <c r="F10" s="40"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
       <c r="I10" s="31"/>
     </row>
     <row r="11" spans="1:10" ht="43.5" customHeight="1" thickBot="1">
       <c r="A11" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="42"/>
+        <v>60</v>
+      </c>
+      <c r="B11" s="41"/>
       <c r="C11" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="41"/>
-      <c r="E11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="41"/>
       <c r="F11" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
       <c r="I11" s="32"/>
     </row>
     <row r="12" spans="1:10" ht="16" thickBot="1">
       <c r="A12" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="42"/>
+      <c r="B12" s="41"/>
       <c r="C12" s="40"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
       <c r="I12" s="33"/>
     </row>
     <row r="13" spans="1:10" ht="16" thickBot="1">
@@ -2721,22 +2721,22 @@
     </row>
     <row r="14" spans="1:10" ht="77.5">
       <c r="A14" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="C14" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="D14" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>81</v>
-      </c>
       <c r="F14" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G14" s="18"/>
       <c r="H14" s="26"/>
@@ -2744,22 +2744,22 @@
     </row>
     <row r="15" spans="1:10" ht="93">
       <c r="A15" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B15" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="C15" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D15" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="E15" s="28" t="s">
-        <v>84</v>
-      </c>
       <c r="F15" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G15" s="28"/>
       <c r="H15" s="29"/>
@@ -2767,22 +2767,22 @@
     </row>
     <row r="16" spans="1:10" ht="78.5" customHeight="1">
       <c r="A16" s="22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B16" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="C16" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>86</v>
-      </c>
       <c r="E16" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G16" s="28"/>
       <c r="H16" s="29"/>
@@ -2791,22 +2791,22 @@
     </row>
     <row r="17" spans="1:10" ht="78.5" customHeight="1">
       <c r="A17" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="29"/>
@@ -2815,22 +2815,22 @@
     </row>
     <row r="18" spans="1:10" ht="75" customHeight="1">
       <c r="A18" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D18" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="E18" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="E18" s="18" t="s">
-        <v>110</v>
-      </c>
       <c r="F18" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G18" s="28"/>
       <c r="H18" s="29"/>
@@ -2839,22 +2839,22 @@
     </row>
     <row r="19" spans="1:10" ht="84" customHeight="1">
       <c r="A19" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="29"/>
@@ -2913,28 +2913,28 @@
       <c r="A24" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="42"/>
+      <c r="B24" s="41"/>
       <c r="C24" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="41"/>
-      <c r="E24" s="42"/>
+        <v>42</v>
+      </c>
+      <c r="D24" s="42"/>
+      <c r="E24" s="41"/>
       <c r="F24" s="16"/>
       <c r="G24" s="17"/>
       <c r="H24" s="17"/>
       <c r="I24" s="32"/>
       <c r="J24" s="23"/>
     </row>
-    <row r="25" spans="1:10" ht="16" thickBot="1">
+    <row r="25" spans="1:10" ht="34" customHeight="1" thickBot="1">
       <c r="A25" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" s="42"/>
+        <v>60</v>
+      </c>
+      <c r="B25" s="41"/>
       <c r="C25" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="41"/>
-      <c r="E25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="41"/>
       <c r="F25" s="16" t="s">
         <v>4</v>
       </c>
@@ -2947,10 +2947,10 @@
       <c r="A26" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="42"/>
+      <c r="B26" s="41"/>
       <c r="C26" s="40"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="41"/>
       <c r="F26" s="16" t="s">
         <v>6</v>
       </c>
@@ -2991,22 +2991,22 @@
     </row>
     <row r="28" spans="1:10" ht="107.5" customHeight="1">
       <c r="A28" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C28" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="E28" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="D28" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="E28" s="28" t="s">
-        <v>96</v>
-      </c>
       <c r="F28" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G28" s="28"/>
       <c r="H28" s="29"/>
@@ -3015,22 +3015,22 @@
     </row>
     <row r="29" spans="1:10" ht="77.5">
       <c r="A29" s="22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B29" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="C29" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="D29" s="28" t="s">
+      <c r="E29" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="E29" s="28" t="s">
-        <v>99</v>
-      </c>
       <c r="F29" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G29" s="28"/>
       <c r="H29" s="29"/>
@@ -3077,28 +3077,28 @@
       <c r="A33" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="42"/>
+      <c r="B33" s="41"/>
       <c r="C33" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="D33" s="41"/>
-      <c r="E33" s="42"/>
+        <v>43</v>
+      </c>
+      <c r="D33" s="42"/>
+      <c r="E33" s="41"/>
       <c r="F33" s="16"/>
       <c r="G33" s="17"/>
       <c r="H33" s="17"/>
       <c r="I33" s="32"/>
       <c r="J33" s="23"/>
     </row>
-    <row r="34" spans="1:10" ht="16" thickBot="1">
+    <row r="34" spans="1:10" ht="41.5" customHeight="1" thickBot="1">
       <c r="A34" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="B34" s="42"/>
+        <v>60</v>
+      </c>
+      <c r="B34" s="41"/>
       <c r="C34" s="40" t="s">
-        <v>100</v>
-      </c>
-      <c r="D34" s="41"/>
-      <c r="E34" s="42"/>
+        <v>99</v>
+      </c>
+      <c r="D34" s="42"/>
+      <c r="E34" s="41"/>
       <c r="F34" s="16" t="s">
         <v>4</v>
       </c>
@@ -3111,10 +3111,10 @@
       <c r="A35" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="42"/>
+      <c r="B35" s="41"/>
       <c r="C35" s="40"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="42"/>
+      <c r="D35" s="42"/>
+      <c r="E35" s="41"/>
       <c r="F35" s="16" t="s">
         <v>6</v>
       </c>
@@ -3155,22 +3155,22 @@
     </row>
     <row r="37" spans="1:10" ht="171.5" customHeight="1">
       <c r="A37" s="22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B37" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="C37" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="C37" s="18" t="s">
+      <c r="D37" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="D37" s="28" t="s">
+      <c r="E37" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="E37" s="28" t="s">
-        <v>106</v>
-      </c>
       <c r="F37" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G37" s="18"/>
       <c r="H37" s="26"/>
@@ -3179,22 +3179,22 @@
     </row>
     <row r="38" spans="1:10" ht="119" customHeight="1">
       <c r="A38" s="22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B38" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="C38" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="C38" s="18" t="s">
-        <v>104</v>
-      </c>
       <c r="D38" s="28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E38" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F38" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G38" s="18"/>
       <c r="H38" s="26"/>
@@ -3203,22 +3203,22 @@
     </row>
     <row r="39" spans="1:10" ht="119" customHeight="1">
       <c r="A39" s="22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B39" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="C39" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="C39" s="18" t="s">
+      <c r="D39" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="E39" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="D39" s="28" t="s">
+      <c r="F39" s="18" t="s">
         <v>119</v>
-      </c>
-      <c r="E39" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="F39" s="18" t="s">
-        <v>120</v>
       </c>
       <c r="G39" s="18"/>
       <c r="H39" s="26"/>
@@ -3227,22 +3227,22 @@
     </row>
     <row r="40" spans="1:10" ht="93">
       <c r="A40" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="B40" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="B40" s="28" t="s">
+      <c r="C40" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="C40" s="18" t="s">
+      <c r="D40" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="E40" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="D40" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="E40" s="28" t="s">
+      <c r="F40" s="18" t="s">
         <v>126</v>
-      </c>
-      <c r="F40" s="18" t="s">
-        <v>127</v>
       </c>
       <c r="G40" s="18"/>
       <c r="H40" s="26"/>
@@ -3277,12 +3277,12 @@
       <c r="A43" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B43" s="42"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="D43" s="41"/>
-      <c r="E43" s="42"/>
+        <v>44</v>
+      </c>
+      <c r="D43" s="42"/>
+      <c r="E43" s="41"/>
       <c r="F43" s="16"/>
       <c r="G43" s="17"/>
       <c r="H43" s="17"/>
@@ -3291,14 +3291,14 @@
     </row>
     <row r="44" spans="1:10" ht="42.5" customHeight="1" thickBot="1">
       <c r="A44" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="B44" s="42"/>
+        <v>60</v>
+      </c>
+      <c r="B44" s="41"/>
       <c r="C44" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="D44" s="41"/>
-      <c r="E44" s="42"/>
+        <v>35</v>
+      </c>
+      <c r="D44" s="42"/>
+      <c r="E44" s="41"/>
       <c r="F44" s="16" t="s">
         <v>4</v>
       </c>
@@ -3311,10 +3311,10 @@
       <c r="A45" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B45" s="42"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="40"/>
-      <c r="D45" s="41"/>
-      <c r="E45" s="42"/>
+      <c r="D45" s="42"/>
+      <c r="E45" s="41"/>
       <c r="F45" s="16" t="s">
         <v>6</v>
       </c>
@@ -3355,22 +3355,22 @@
     </row>
     <row r="47" spans="1:10" ht="192.5" customHeight="1">
       <c r="A47" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="B47" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="B47" s="28" t="s">
+      <c r="C47" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="D47" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="C47" s="18" t="s">
+      <c r="E47" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="D47" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="E47" s="28" t="s">
-        <v>132</v>
-      </c>
       <c r="F47" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G47" s="18"/>
       <c r="H47" s="26"/>
@@ -3379,22 +3379,22 @@
     </row>
     <row r="48" spans="1:10" ht="202.5" customHeight="1">
       <c r="A48" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="B48" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="B48" s="28" t="s">
-        <v>129</v>
-      </c>
       <c r="C48" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D48" s="28" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E48" s="28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F48" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G48" s="18"/>
       <c r="H48" s="26"/>
@@ -3403,22 +3403,22 @@
     </row>
     <row r="49" spans="1:10" ht="170.5">
       <c r="A49" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="B49" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="B49" s="28" t="s">
-        <v>129</v>
-      </c>
       <c r="C49" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D49" s="28" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E49" s="28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F49" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G49" s="18"/>
       <c r="H49" s="26"/>
@@ -3427,22 +3427,22 @@
     </row>
     <row r="50" spans="1:10" ht="155">
       <c r="A50" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="B50" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="B50" s="28" t="s">
-        <v>124</v>
-      </c>
       <c r="C50" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="D50" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="D50" s="28" t="s">
+      <c r="E50" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="E50" s="28" t="s">
-        <v>139</v>
-      </c>
       <c r="F50" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G50" s="18"/>
       <c r="H50" s="26"/>
@@ -3477,12 +3477,12 @@
       <c r="A53" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B53" s="42"/>
+      <c r="B53" s="41"/>
       <c r="C53" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="D53" s="41"/>
-      <c r="E53" s="42"/>
+        <v>45</v>
+      </c>
+      <c r="D53" s="42"/>
+      <c r="E53" s="41"/>
       <c r="F53" s="16"/>
       <c r="G53" s="17"/>
       <c r="H53" s="17"/>
@@ -3491,14 +3491,14 @@
     </row>
     <row r="54" spans="1:10" ht="16" thickBot="1">
       <c r="A54" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="B54" s="42"/>
+        <v>60</v>
+      </c>
+      <c r="B54" s="41"/>
       <c r="C54" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="D54" s="41"/>
-      <c r="E54" s="42"/>
+        <v>36</v>
+      </c>
+      <c r="D54" s="42"/>
+      <c r="E54" s="41"/>
       <c r="F54" s="16" t="s">
         <v>4</v>
       </c>
@@ -3511,10 +3511,10 @@
       <c r="A55" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B55" s="42"/>
+      <c r="B55" s="41"/>
       <c r="C55" s="40"/>
-      <c r="D55" s="41"/>
-      <c r="E55" s="42"/>
+      <c r="D55" s="42"/>
+      <c r="E55" s="41"/>
       <c r="F55" s="16" t="s">
         <v>6</v>
       </c>
@@ -3555,22 +3555,22 @@
     </row>
     <row r="57" spans="1:10" ht="62">
       <c r="A57" s="22" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B57" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="C57" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="C57" s="18" t="s">
+      <c r="D57" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="E57" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="D57" s="28" t="s">
-        <v>149</v>
-      </c>
-      <c r="E57" s="28" t="s">
-        <v>142</v>
-      </c>
       <c r="F57" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G57" s="18"/>
       <c r="H57" s="26"/>
@@ -3579,22 +3579,22 @@
     </row>
     <row r="58" spans="1:10" ht="62">
       <c r="A58" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="B58" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="C58" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="D58" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="B58" s="28" t="s">
+      <c r="E58" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="C58" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="D58" s="28" t="s">
-        <v>149</v>
-      </c>
-      <c r="E58" s="28" t="s">
-        <v>144</v>
-      </c>
       <c r="F58" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G58" s="18"/>
       <c r="H58" s="26"/>
@@ -3629,12 +3629,12 @@
       <c r="A61" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B61" s="42"/>
+      <c r="B61" s="41"/>
       <c r="C61" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="D61" s="41"/>
-      <c r="E61" s="42"/>
+        <v>46</v>
+      </c>
+      <c r="D61" s="42"/>
+      <c r="E61" s="41"/>
       <c r="F61" s="16"/>
       <c r="G61" s="17"/>
       <c r="H61" s="17"/>
@@ -3643,14 +3643,14 @@
     </row>
     <row r="62" spans="1:10" ht="38.5" customHeight="1" thickBot="1">
       <c r="A62" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="B62" s="42"/>
+        <v>60</v>
+      </c>
+      <c r="B62" s="41"/>
       <c r="C62" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="D62" s="41"/>
-      <c r="E62" s="42"/>
+      <c r="D62" s="42"/>
+      <c r="E62" s="41"/>
       <c r="F62" s="16" t="s">
         <v>4</v>
       </c>
@@ -3663,10 +3663,10 @@
       <c r="A63" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B63" s="42"/>
+      <c r="B63" s="41"/>
       <c r="C63" s="40"/>
-      <c r="D63" s="41"/>
-      <c r="E63" s="42"/>
+      <c r="D63" s="42"/>
+      <c r="E63" s="41"/>
       <c r="F63" s="16" t="s">
         <v>6</v>
       </c>
@@ -3707,22 +3707,22 @@
     </row>
     <row r="65" spans="1:10" ht="68.5" customHeight="1">
       <c r="A65" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B65" s="28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C65" s="18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D65" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="E65" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="E65" s="28" t="s">
-        <v>151</v>
-      </c>
       <c r="F65" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G65" s="18"/>
       <c r="H65" s="26"/>
@@ -7025,33 +7025,11 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:E25"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="C33:E33"/>
@@ -7068,11 +7046,33 @@
     <mergeCell ref="C11:E11"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="C63:E63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7101,7 +7101,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" s="38"/>
     </row>
@@ -7110,7 +7110,7 @@
         <v>16</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="38"/>
     </row>
@@ -7119,7 +7119,7 @@
         <v>17</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" s="38"/>
     </row>
@@ -7142,7 +7142,7 @@
       <c r="D6" s="38"/>
     </row>
     <row r="7" spans="2:7" ht="13" thickTop="1"/>
-    <row r="8" spans="2:7" s="10" customFormat="1" ht="43.5">
+    <row r="8" spans="2:7" s="10" customFormat="1" ht="29">
       <c r="B8" s="8" t="s">
         <v>20</v>
       </c>
@@ -7153,7 +7153,7 @@
         <v>22</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>23</v>
@@ -7164,16 +7164,16 @@
     </row>
     <row r="9" spans="2:7" ht="25" customHeight="1">
       <c r="B9" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>0</v>
@@ -7184,16 +7184,16 @@
     </row>
     <row r="10" spans="2:7" ht="30" customHeight="1">
       <c r="B10" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D10" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="15" t="s">
         <v>52</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>53</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>1</v>
@@ -7202,16 +7202,16 @@
     </row>
     <row r="11" spans="2:7" ht="30.5" customHeight="1">
       <c r="B11" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>1</v>
@@ -7222,16 +7222,16 @@
     </row>
     <row r="12" spans="2:7" ht="32" customHeight="1">
       <c r="B12" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D12" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="14" t="s">
         <v>55</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>56</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>0</v>
@@ -7242,16 +7242,16 @@
     </row>
     <row r="13" spans="2:7" ht="23" customHeight="1">
       <c r="B13" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C13" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="14" t="s">
-        <v>59</v>
-      </c>
       <c r="E13" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>0</v>
@@ -7374,12 +7374,12 @@
       <c r="A1" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="42"/>
+      <c r="B1" s="41"/>
       <c r="C1" s="40" t="s">
-        <v>153</v>
-      </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="42"/>
+        <v>152</v>
+      </c>
+      <c r="D1" s="42"/>
+      <c r="E1" s="41"/>
       <c r="F1" s="16"/>
       <c r="G1" s="17"/>
       <c r="H1" s="17"/>
@@ -7387,14 +7387,14 @@
     </row>
     <row r="2" spans="1:9" ht="16" thickBot="1">
       <c r="A2" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="42"/>
+        <v>60</v>
+      </c>
+      <c r="B2" s="41"/>
       <c r="C2" s="40" t="s">
-        <v>152</v>
-      </c>
-      <c r="D2" s="41"/>
-      <c r="E2" s="42"/>
+        <v>151</v>
+      </c>
+      <c r="D2" s="42"/>
+      <c r="E2" s="41"/>
       <c r="F2" s="16" t="s">
         <v>4</v>
       </c>
@@ -7406,10 +7406,10 @@
       <c r="A3" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="42"/>
+      <c r="B3" s="41"/>
       <c r="C3" s="40"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="41"/>
       <c r="F3" s="16" t="s">
         <v>6</v>
       </c>
@@ -7448,22 +7448,22 @@
     </row>
     <row r="5" spans="1:9" ht="62">
       <c r="A5" s="22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B5" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="D5" s="28" t="s">
         <v>158</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="E5" s="28" t="s">
         <v>159</v>
       </c>
-      <c r="E5" s="28" t="s">
-        <v>160</v>
-      </c>
       <c r="F5" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G5" s="18"/>
       <c r="H5" s="26"/>
@@ -7474,12 +7474,12 @@
       <c r="A8" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="42"/>
+      <c r="B8" s="41"/>
       <c r="C8" s="40" t="s">
-        <v>154</v>
-      </c>
-      <c r="D8" s="41"/>
-      <c r="E8" s="42"/>
+        <v>153</v>
+      </c>
+      <c r="D8" s="42"/>
+      <c r="E8" s="41"/>
       <c r="F8" s="16"/>
       <c r="G8" s="17"/>
       <c r="H8" s="17"/>
@@ -7487,14 +7487,14 @@
     </row>
     <row r="9" spans="1:9" ht="16" thickBot="1">
       <c r="A9" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="42"/>
+        <v>60</v>
+      </c>
+      <c r="B9" s="41"/>
       <c r="C9" s="40" t="s">
-        <v>166</v>
-      </c>
-      <c r="D9" s="41"/>
-      <c r="E9" s="42"/>
+        <v>165</v>
+      </c>
+      <c r="D9" s="42"/>
+      <c r="E9" s="41"/>
       <c r="F9" s="16" t="s">
         <v>4</v>
       </c>
@@ -7506,10 +7506,10 @@
       <c r="A10" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="42"/>
+      <c r="B10" s="41"/>
       <c r="C10" s="40"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="41"/>
       <c r="F10" s="16" t="s">
         <v>6</v>
       </c>
@@ -7548,22 +7548,22 @@
     </row>
     <row r="12" spans="1:9" ht="97.5" customHeight="1">
       <c r="A12" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="C12" s="18" t="s">
         <v>162</v>
       </c>
-      <c r="B12" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="C12" s="18" t="s">
+      <c r="D12" s="28" t="s">
         <v>163</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="E12" s="28" t="s">
         <v>164</v>
       </c>
-      <c r="E12" s="28" t="s">
-        <v>165</v>
-      </c>
       <c r="F12" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G12" s="18"/>
       <c r="H12" s="26"/>
@@ -7574,12 +7574,12 @@
       <c r="A15" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="42"/>
+      <c r="B15" s="41"/>
       <c r="C15" s="40" t="s">
-        <v>156</v>
-      </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="42"/>
+        <v>155</v>
+      </c>
+      <c r="D15" s="42"/>
+      <c r="E15" s="41"/>
       <c r="F15" s="16"/>
       <c r="G15" s="17"/>
       <c r="H15" s="17"/>
@@ -7587,14 +7587,14 @@
     </row>
     <row r="16" spans="1:9" ht="39.5" customHeight="1" thickBot="1">
       <c r="A16" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="42"/>
+        <v>60</v>
+      </c>
+      <c r="B16" s="41"/>
       <c r="C16" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="41"/>
-      <c r="E16" s="42"/>
+        <v>59</v>
+      </c>
+      <c r="D16" s="42"/>
+      <c r="E16" s="41"/>
       <c r="F16" s="16" t="s">
         <v>4</v>
       </c>
@@ -7606,10 +7606,10 @@
       <c r="A17" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="42"/>
+      <c r="B17" s="41"/>
       <c r="C17" s="40"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="41"/>
       <c r="F17" s="16" t="s">
         <v>6</v>
       </c>
@@ -7648,22 +7648,22 @@
     </row>
     <row r="19" spans="1:9" ht="146.5" customHeight="1">
       <c r="A19" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="D19" s="28" t="s">
         <v>168</v>
       </c>
-      <c r="B19" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="D19" s="28" t="s">
+      <c r="E19" s="28" t="s">
         <v>169</v>
       </c>
-      <c r="E19" s="28" t="s">
-        <v>170</v>
-      </c>
       <c r="F19" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G19" s="18"/>
       <c r="H19" s="26"/>
@@ -7674,12 +7674,12 @@
       <c r="A22" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="42"/>
+      <c r="B22" s="41"/>
       <c r="C22" s="40" t="s">
-        <v>155</v>
-      </c>
-      <c r="D22" s="41"/>
-      <c r="E22" s="42"/>
+        <v>154</v>
+      </c>
+      <c r="D22" s="42"/>
+      <c r="E22" s="41"/>
       <c r="F22" s="16"/>
       <c r="G22" s="17"/>
       <c r="H22" s="17"/>
@@ -7687,14 +7687,14 @@
     </row>
     <row r="23" spans="1:9" ht="16" thickBot="1">
       <c r="A23" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" s="42"/>
+        <v>60</v>
+      </c>
+      <c r="B23" s="41"/>
       <c r="C23" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="D23" s="41"/>
-      <c r="E23" s="42"/>
+        <v>54</v>
+      </c>
+      <c r="D23" s="42"/>
+      <c r="E23" s="41"/>
       <c r="F23" s="16" t="s">
         <v>4</v>
       </c>
@@ -7706,10 +7706,10 @@
       <c r="A24" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="42"/>
+      <c r="B24" s="41"/>
       <c r="C24" s="40"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="41"/>
       <c r="F24" s="16" t="s">
         <v>6</v>
       </c>
@@ -7748,22 +7748,22 @@
     </row>
     <row r="26" spans="1:9" ht="139.5">
       <c r="A26" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="C26" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="B26" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="C26" s="18" t="s">
+      <c r="D26" s="28" t="s">
         <v>172</v>
       </c>
-      <c r="D26" s="28" t="s">
+      <c r="E26" s="28" t="s">
         <v>173</v>
       </c>
-      <c r="E26" s="28" t="s">
-        <v>174</v>
-      </c>
       <c r="F26" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G26" s="18"/>
       <c r="H26" s="26"/>
@@ -7774,12 +7774,12 @@
       <c r="A29" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="42"/>
+      <c r="B29" s="41"/>
       <c r="C29" s="40" t="s">
-        <v>175</v>
-      </c>
-      <c r="D29" s="41"/>
-      <c r="E29" s="42"/>
+        <v>174</v>
+      </c>
+      <c r="D29" s="42"/>
+      <c r="E29" s="41"/>
       <c r="F29" s="16"/>
       <c r="G29" s="17"/>
       <c r="H29" s="17"/>
@@ -7787,14 +7787,14 @@
     </row>
     <row r="30" spans="1:9" ht="16" thickBot="1">
       <c r="A30" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="B30" s="42"/>
+        <v>60</v>
+      </c>
+      <c r="B30" s="41"/>
       <c r="C30" s="40" t="s">
-        <v>176</v>
-      </c>
-      <c r="D30" s="41"/>
-      <c r="E30" s="42"/>
+        <v>175</v>
+      </c>
+      <c r="D30" s="42"/>
+      <c r="E30" s="41"/>
       <c r="F30" s="16" t="s">
         <v>4</v>
       </c>
@@ -7806,10 +7806,10 @@
       <c r="A31" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B31" s="42"/>
+      <c r="B31" s="41"/>
       <c r="C31" s="40"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="41"/>
       <c r="F31" s="16" t="s">
         <v>6</v>
       </c>
@@ -7848,22 +7848,22 @@
     </row>
     <row r="33" spans="1:9" ht="124">
       <c r="A33" s="22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B33" s="28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C33" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="D33" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="E33" s="28" t="s">
         <v>177</v>
       </c>
-      <c r="D33" s="28" t="s">
-        <v>173</v>
-      </c>
-      <c r="E33" s="28" t="s">
-        <v>178</v>
-      </c>
       <c r="F33" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G33" s="18"/>
       <c r="H33" s="26"/>
@@ -7871,36 +7871,36 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:E24"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="C29:E29"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="C31:E31"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>